<commit_message>
Caso final T_PT5:FINAL hotfix1
</commit_message>
<xml_diff>
--- a/caso_final/casofinal_excel (2).xlsx
+++ b/caso_final/casofinal_excel (2).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\belen\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\jujor\OperaDownloadFolder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A317154-24C1-4028-80F5-7F6AB5AF4309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F87D7027-B396-4217-8DDB-82EDF77ED5DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="313">
   <si>
     <t>patient_id</t>
   </si>
@@ -617,9 +617,6 @@
     <t>(S5, #p#82, sk11)</t>
   </si>
   <si>
-    <t>(S6, #p#75, sk12)</t>
-  </si>
-  <si>
     <t>(S6, #p#99, sk3)</t>
   </si>
   <si>
@@ -659,9 +656,6 @@
     <t>(S6, #p#70, sk12)</t>
   </si>
   <si>
-    <t>(S1, #p#69, sk6)</t>
-  </si>
-  <si>
     <t>(S1, #p#10, sk7)</t>
   </si>
   <si>
@@ -683,9 +677,6 @@
     <t>(S6, #p#47, sk12)</t>
   </si>
   <si>
-    <t>(S5, #p#63, sk12)</t>
-  </si>
-  <si>
     <t>(S3, #p#31, sk6)</t>
   </si>
   <si>
@@ -698,15 +689,9 @@
     <t>S_OR4</t>
   </si>
   <si>
-    <t>(S1, #p#20, sk5)</t>
-  </si>
-  <si>
     <t>(S2, #p#80, sk5)</t>
   </si>
   <si>
-    <t>(S4, #p#9, sk5)</t>
-  </si>
-  <si>
     <t>(S3, #p#85, sk9)</t>
   </si>
   <si>
@@ -719,18 +704,9 @@
     <t>(S4, #p#8, sk8)</t>
   </si>
   <si>
-    <t>(S4, #p#28, sk2)</t>
-  </si>
-  <si>
-    <t>(S2, #p#90, sk5)</t>
-  </si>
-  <si>
     <t>(S1, #p#48, sk5)</t>
   </si>
   <si>
-    <t>(S2, #p#38, sk5)</t>
-  </si>
-  <si>
     <t>(S4, #p#12, sk8)</t>
   </si>
   <si>
@@ -740,12 +716,6 @@
     <t>(S2, #p#40, sk2)</t>
   </si>
   <si>
-    <t>(S2, #p#36, sk2)</t>
-  </si>
-  <si>
-    <t>(S3, #p#37, sk4)</t>
-  </si>
-  <si>
     <t>(S2, #p#16, sk5)</t>
   </si>
   <si>
@@ -755,9 +725,6 @@
     <t>(S4, #p#55, sk5)</t>
   </si>
   <si>
-    <t>(S4, #p#46, sk10)</t>
-  </si>
-  <si>
     <t>(S3, #p#41, sk9)</t>
   </si>
   <si>
@@ -938,13 +905,67 @@
     <t>Cirujano</t>
   </si>
   <si>
-    <t>Dolencia</t>
-  </si>
-  <si>
     <t>Carga trabajo</t>
   </si>
   <si>
     <t>18h</t>
+  </si>
+  <si>
+    <t>Cirujano que opera</t>
+  </si>
+  <si>
+    <t>Dolencia a operar</t>
+  </si>
+  <si>
+    <t>(S1, #p#38, sk5)</t>
+  </si>
+  <si>
+    <t>(S2, #p#9, sk5)</t>
+  </si>
+  <si>
+    <t>(S1, #p#90, sk5)</t>
+  </si>
+  <si>
+    <t>(S4, #p#20, sk5)</t>
+  </si>
+  <si>
+    <t>(S5, #p#75, sk12)</t>
+  </si>
+  <si>
+    <t>(S3, #p#69, sk6)</t>
+  </si>
+  <si>
+    <t>(S6, #p#63, sk12)</t>
+  </si>
+  <si>
+    <t>(S4, #p#36, sk2)</t>
+  </si>
+  <si>
+    <t>(S2, #p#46, sk10)</t>
+  </si>
+  <si>
+    <t>(S4, #p#37, sk4)</t>
+  </si>
+  <si>
+    <t>(S2, #p#28, sk2)</t>
+  </si>
+  <si>
+    <t>(OR3, #p#38, sk5)</t>
+  </si>
+  <si>
+    <t>(OR1, #p#27, sk7)</t>
+  </si>
+  <si>
+    <t>(OR3, #p#9, sk5)</t>
+  </si>
+  <si>
+    <t>(OR2, #p#31, sk6)</t>
+  </si>
+  <si>
+    <t>(OR1, #p#86, sk11)</t>
+  </si>
+  <si>
+    <t>(OR1, #p#26, sk3)</t>
   </si>
 </sst>
 </file>
@@ -1129,7 +1150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1162,7 +1183,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1178,8 +1198,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1527,15 +1545,15 @@
       <selection activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1549,7 +1567,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1563,7 +1581,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1577,7 +1595,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1591,7 +1609,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1605,7 +1623,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1619,7 +1637,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1633,7 +1651,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1647,7 +1665,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1661,7 +1679,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1675,7 +1693,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1689,7 +1707,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -1703,7 +1721,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1717,7 +1735,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1731,7 +1749,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -1745,7 +1763,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -1759,7 +1777,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -1773,7 +1791,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -1787,7 +1805,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -1801,7 +1819,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -1815,7 +1833,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -1829,7 +1847,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -1843,7 +1861,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -1857,7 +1875,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -1871,7 +1889,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>38</v>
       </c>
@@ -1885,7 +1903,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -1899,7 +1917,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -1913,7 +1931,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>41</v>
       </c>
@@ -1927,7 +1945,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -1941,7 +1959,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>43</v>
       </c>
@@ -1955,7 +1973,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>44</v>
       </c>
@@ -1969,7 +1987,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>45</v>
       </c>
@@ -1983,7 +2001,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>46</v>
       </c>
@@ -1997,7 +2015,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>47</v>
       </c>
@@ -2011,7 +2029,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>48</v>
       </c>
@@ -2025,7 +2043,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>49</v>
       </c>
@@ -2039,7 +2057,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>50</v>
       </c>
@@ -2053,7 +2071,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>51</v>
       </c>
@@ -2067,7 +2085,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>52</v>
       </c>
@@ -2081,7 +2099,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>53</v>
       </c>
@@ -2095,7 +2113,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>54</v>
       </c>
@@ -2109,7 +2127,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>55</v>
       </c>
@@ -2123,7 +2141,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>56</v>
       </c>
@@ -2137,7 +2155,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>57</v>
       </c>
@@ -2151,7 +2169,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>58</v>
       </c>
@@ -2165,7 +2183,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>59</v>
       </c>
@@ -2179,7 +2197,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>60</v>
       </c>
@@ -2193,7 +2211,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>61</v>
       </c>
@@ -2207,7 +2225,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>63</v>
       </c>
@@ -2221,7 +2239,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>64</v>
       </c>
@@ -2235,7 +2253,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>65</v>
       </c>
@@ -2249,7 +2267,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>66</v>
       </c>
@@ -2263,7 +2281,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>67</v>
       </c>
@@ -2277,7 +2295,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>68</v>
       </c>
@@ -2291,7 +2309,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>69</v>
       </c>
@@ -2305,7 +2323,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>70</v>
       </c>
@@ -2319,7 +2337,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>71</v>
       </c>
@@ -2333,7 +2351,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>72</v>
       </c>
@@ -2347,7 +2365,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>73</v>
       </c>
@@ -2361,7 +2379,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>74</v>
       </c>
@@ -2375,7 +2393,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>75</v>
       </c>
@@ -2389,7 +2407,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>76</v>
       </c>
@@ -2403,7 +2421,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>77</v>
       </c>
@@ -2417,7 +2435,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>78</v>
       </c>
@@ -2431,7 +2449,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>79</v>
       </c>
@@ -2445,7 +2463,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>80</v>
       </c>
@@ -2459,7 +2477,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>81</v>
       </c>
@@ -2473,7 +2491,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>82</v>
       </c>
@@ -2487,7 +2505,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>83</v>
       </c>
@@ -2501,7 +2519,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>84</v>
       </c>
@@ -2515,7 +2533,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>85</v>
       </c>
@@ -2529,7 +2547,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>86</v>
       </c>
@@ -2543,7 +2561,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>87</v>
       </c>
@@ -2557,7 +2575,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>88</v>
       </c>
@@ -2571,7 +2589,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>89</v>
       </c>
@@ -2585,7 +2603,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>90</v>
       </c>
@@ -2599,7 +2617,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>91</v>
       </c>
@@ -2613,7 +2631,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>92</v>
       </c>
@@ -2627,7 +2645,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>93</v>
       </c>
@@ -2641,7 +2659,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>94</v>
       </c>
@@ -2655,7 +2673,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>95</v>
       </c>
@@ -2669,7 +2687,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>96</v>
       </c>
@@ -2683,7 +2701,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>97</v>
       </c>
@@ -2697,7 +2715,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>98</v>
       </c>
@@ -2711,7 +2729,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>99</v>
       </c>
@@ -2725,7 +2743,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>100</v>
       </c>
@@ -2739,7 +2757,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>101</v>
       </c>
@@ -2753,7 +2771,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>102</v>
       </c>
@@ -2767,7 +2785,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>103</v>
       </c>
@@ -2781,7 +2799,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>104</v>
       </c>
@@ -2795,7 +2813,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>105</v>
       </c>
@@ -2809,7 +2827,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>106</v>
       </c>
@@ -2823,7 +2841,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>107</v>
       </c>
@@ -2837,7 +2855,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>108</v>
       </c>
@@ -2851,7 +2869,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>109</v>
       </c>
@@ -2865,7 +2883,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>110</v>
       </c>
@@ -2879,7 +2897,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>111</v>
       </c>
@@ -2893,7 +2911,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>112</v>
       </c>
@@ -2907,7 +2925,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>113</v>
       </c>
@@ -2921,7 +2939,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>114</v>
       </c>
@@ -2935,7 +2953,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>115</v>
       </c>
@@ -2963,23 +2981,23 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" customWidth="1"/>
     <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.88671875" customWidth="1"/>
-    <col min="4" max="11" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.85546875" customWidth="1"/>
+    <col min="4" max="11" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="4.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C3" s="4" t="s">
         <v>116</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>117</v>
       </c>
@@ -3020,7 +3038,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>118</v>
       </c>
@@ -3064,7 +3082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
         <v>120</v>
       </c>
@@ -3105,7 +3123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>121</v>
       </c>
@@ -3146,7 +3164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
         <v>122</v>
       </c>
@@ -3187,7 +3205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
         <v>123</v>
       </c>
@@ -3228,7 +3246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
         <v>124</v>
       </c>
@@ -3269,9 +3287,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -3323,13 +3341,13 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="10" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="10" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="4.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>125</v>
       </c>
@@ -3370,7 +3388,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>126</v>
       </c>
@@ -3384,7 +3402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>127</v>
       </c>
@@ -3401,7 +3419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>128</v>
       </c>
@@ -3409,7 +3427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>129</v>
       </c>
@@ -3445,24 +3463,24 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>133</v>
       </c>
@@ -3480,34 +3498,34 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>139</v>
       </c>
@@ -3521,679 +3539,679 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B3:H105"/>
   <sheetViews>
-    <sheetView topLeftCell="B5" zoomScale="94" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+    <sheetView topLeftCell="A76" zoomScale="94" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M71" sqref="M71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="7.109375" customWidth="1"/>
-    <col min="5" max="5" width="7.6640625" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" customWidth="1"/>
-    <col min="7" max="7" width="8.44140625" customWidth="1"/>
-    <col min="8" max="8" width="7.77734375" customWidth="1"/>
-    <col min="9" max="9" width="9.21875" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="22" t="s">
+    <row r="3" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B3" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="C3" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="22" t="s">
+      <c r="C3" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="19" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="22" t="s">
+    <row r="4" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="23">
-        <v>1</v>
-      </c>
-      <c r="D4" s="24" t="s">
+      <c r="C4" s="20">
+        <v>1</v>
+      </c>
+      <c r="D4" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="21" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="22" t="s">
+    <row r="5" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="23">
-        <v>1</v>
-      </c>
-      <c r="D5" s="24" t="s">
+      <c r="C5" s="20">
+        <v>1</v>
+      </c>
+      <c r="D5" s="21" t="s">
         <v>141</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="21" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="22" t="s">
+    <row r="6" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="23">
-        <v>2</v>
-      </c>
-      <c r="D6" s="24" t="s">
+      <c r="C6" s="20">
+        <v>2</v>
+      </c>
+      <c r="D6" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="21" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B7" s="22" t="s">
+    <row r="7" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B7" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="23">
-        <v>2</v>
-      </c>
-      <c r="D7" s="24" t="s">
+      <c r="C7" s="20">
+        <v>2</v>
+      </c>
+      <c r="D7" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="21" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B8" s="22" t="s">
+    <row r="8" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="23">
-        <v>1</v>
-      </c>
-      <c r="D8" s="24" t="s">
+      <c r="C8" s="20">
+        <v>1</v>
+      </c>
+      <c r="D8" s="21" t="s">
         <v>144</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="21" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B9" s="22" t="s">
+    <row r="9" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="23">
-        <v>1</v>
-      </c>
-      <c r="D9" s="24" t="s">
+      <c r="C9" s="20">
+        <v>1</v>
+      </c>
+      <c r="D9" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="21" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B10" s="22" t="s">
+    <row r="10" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="23">
-        <v>2</v>
-      </c>
-      <c r="D10" s="24" t="s">
+      <c r="C10" s="20">
+        <v>2</v>
+      </c>
+      <c r="D10" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B11" s="22" t="s">
+    <row r="11" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="23">
-        <v>1</v>
-      </c>
-      <c r="D11" s="24" t="s">
+      <c r="C11" s="20">
+        <v>1</v>
+      </c>
+      <c r="D11" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="E11" s="21" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B12" s="22" t="s">
+    <row r="12" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B12" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="23">
-        <v>1</v>
-      </c>
-      <c r="D12" s="24" t="s">
+      <c r="C12" s="20">
+        <v>1</v>
+      </c>
+      <c r="D12" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="E12" s="21" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B13" s="22" t="s">
+    <row r="13" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="23">
-        <v>1</v>
-      </c>
-      <c r="D13" s="24" t="s">
+      <c r="C13" s="20">
+        <v>1</v>
+      </c>
+      <c r="D13" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="E13" s="24" t="s">
+      <c r="E13" s="21" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B14" s="22" t="s">
+    <row r="14" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="23">
-        <v>1</v>
-      </c>
-      <c r="D14" s="24" t="s">
+      <c r="C14" s="20">
+        <v>1</v>
+      </c>
+      <c r="D14" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="E14" s="24" t="s">
+      <c r="E14" s="21" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B15" s="22" t="s">
+    <row r="15" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B15" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="23">
-        <v>1</v>
-      </c>
-      <c r="D15" s="24" t="s">
+      <c r="C15" s="20">
+        <v>1</v>
+      </c>
+      <c r="D15" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="E15" s="24" t="s">
+      <c r="E15" s="21" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B16" s="22" t="s">
+    <row r="16" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="23">
-        <v>1</v>
-      </c>
-      <c r="D16" s="24" t="s">
+      <c r="C16" s="20">
+        <v>1</v>
+      </c>
+      <c r="D16" s="21" t="s">
         <v>152</v>
       </c>
-      <c r="E16" s="24" t="s">
+      <c r="E16" s="21" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B17" s="22" t="s">
+    <row r="17" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B17" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="23">
-        <v>1</v>
-      </c>
-      <c r="D17" s="24" t="s">
+      <c r="C17" s="20">
+        <v>1</v>
+      </c>
+      <c r="D17" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="E17" s="24" t="s">
+      <c r="E17" s="21" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B18" s="22" t="s">
+    <row r="18" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="23">
-        <v>1</v>
-      </c>
-      <c r="D18" s="24" t="s">
+      <c r="C18" s="20">
+        <v>1</v>
+      </c>
+      <c r="D18" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="E18" s="24" t="s">
+      <c r="E18" s="21" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B19" s="22" t="s">
+    <row r="19" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B19" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="23">
-        <v>1</v>
-      </c>
-      <c r="D19" s="24" t="s">
+      <c r="C19" s="20">
+        <v>1</v>
+      </c>
+      <c r="D19" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="E19" s="24" t="s">
+      <c r="E19" s="21" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B20" s="22" t="s">
+    <row r="20" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B20" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="23">
-        <v>1</v>
-      </c>
-      <c r="D20" s="24" t="s">
+      <c r="C20" s="20">
+        <v>1</v>
+      </c>
+      <c r="D20" s="21" t="s">
         <v>156</v>
       </c>
-      <c r="E20" s="24" t="s">
+      <c r="E20" s="21" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B21" s="22" t="s">
+    <row r="21" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B21" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="23">
-        <v>1</v>
-      </c>
-      <c r="D21" s="24" t="s">
+      <c r="C21" s="20">
+        <v>1</v>
+      </c>
+      <c r="D21" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="E21" s="24" t="s">
+      <c r="E21" s="21" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="22" t="s">
+    <row r="22" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B22" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="C22" s="23">
-        <v>1</v>
-      </c>
-      <c r="D22" s="24" t="s">
+      <c r="C22" s="20">
+        <v>1</v>
+      </c>
+      <c r="D22" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="E22" s="24" t="s">
+      <c r="E22" s="21" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B23" s="22" t="s">
+    <row r="23" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B23" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C23" s="23">
-        <v>1</v>
-      </c>
-      <c r="D23" s="24" t="s">
+      <c r="C23" s="20">
+        <v>1</v>
+      </c>
+      <c r="D23" s="21" t="s">
         <v>159</v>
       </c>
-      <c r="E23" s="24" t="s">
+      <c r="E23" s="21" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B24" s="22" t="s">
+    <row r="24" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B24" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="C24" s="23">
-        <v>1</v>
-      </c>
-      <c r="D24" s="24" t="s">
+      <c r="C24" s="20">
+        <v>1</v>
+      </c>
+      <c r="D24" s="21" t="s">
         <v>160</v>
       </c>
-      <c r="E24" s="24" t="s">
+      <c r="E24" s="21" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B25" s="22" t="s">
+    <row r="25" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B25" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="C25" s="23">
-        <v>1</v>
-      </c>
-      <c r="D25" s="24" t="s">
+      <c r="C25" s="20">
+        <v>1</v>
+      </c>
+      <c r="D25" s="21" t="s">
         <v>161</v>
       </c>
-      <c r="E25" s="24" t="s">
+      <c r="E25" s="21" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B26" s="22" t="s">
+    <row r="26" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B26" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="C26" s="23">
-        <v>1</v>
-      </c>
-      <c r="D26" s="24" t="s">
+      <c r="C26" s="20">
+        <v>1</v>
+      </c>
+      <c r="D26" s="21" t="s">
         <v>162</v>
       </c>
-      <c r="E26" s="24" t="s">
+      <c r="E26" s="21" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B27" s="22" t="s">
+    <row r="27" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B27" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="C27" s="23">
-        <v>1</v>
-      </c>
-      <c r="D27" s="24" t="s">
+      <c r="C27" s="20">
+        <v>1</v>
+      </c>
+      <c r="D27" s="21" t="s">
         <v>163</v>
       </c>
-      <c r="E27" s="24" t="s">
+      <c r="E27" s="21" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B28" s="22" t="s">
+    <row r="28" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B28" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="C28" s="23">
-        <v>1</v>
-      </c>
-      <c r="D28" s="24" t="s">
+      <c r="C28" s="20">
+        <v>1</v>
+      </c>
+      <c r="D28" s="21" t="s">
         <v>164</v>
       </c>
-      <c r="E28" s="24" t="s">
+      <c r="E28" s="21" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B29" s="22" t="s">
+    <row r="29" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B29" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="C29" s="23">
-        <v>1</v>
-      </c>
-      <c r="D29" s="24" t="s">
+      <c r="C29" s="20">
+        <v>1</v>
+      </c>
+      <c r="D29" s="21" t="s">
         <v>165</v>
       </c>
-      <c r="E29" s="24" t="s">
+      <c r="E29" s="21" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B30" s="22" t="s">
+    <row r="30" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B30" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="C30" s="23">
-        <v>2</v>
-      </c>
-      <c r="D30" s="24" t="s">
+      <c r="C30" s="20">
+        <v>2</v>
+      </c>
+      <c r="D30" s="21" t="s">
         <v>166</v>
       </c>
-      <c r="E30" s="24" t="s">
+      <c r="E30" s="21" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B31" s="22" t="s">
+    <row r="31" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B31" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="C31" s="23">
-        <v>1</v>
-      </c>
-      <c r="D31" s="24" t="s">
+      <c r="C31" s="20">
+        <v>1</v>
+      </c>
+      <c r="D31" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="E31" s="24" t="s">
+      <c r="E31" s="21" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B32" s="22" t="s">
+    <row r="32" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B32" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="C32" s="23">
-        <v>2</v>
-      </c>
-      <c r="D32" s="24" t="s">
+      <c r="C32" s="20">
+        <v>2</v>
+      </c>
+      <c r="D32" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="E32" s="24" t="s">
+      <c r="E32" s="21" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B33" s="22" t="s">
+    <row r="33" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B33" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="C33" s="23">
-        <v>1</v>
-      </c>
-      <c r="D33" s="24" t="s">
+      <c r="C33" s="20">
+        <v>1</v>
+      </c>
+      <c r="D33" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="E33" s="24" t="s">
+      <c r="E33" s="21" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B34" s="22" t="s">
+    <row r="34" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B34" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="C34" s="23">
-        <v>1</v>
-      </c>
-      <c r="D34" s="24" t="s">
+      <c r="C34" s="20">
+        <v>1</v>
+      </c>
+      <c r="D34" s="21" t="s">
         <v>170</v>
       </c>
-      <c r="E34" s="24" t="s">
+      <c r="E34" s="21" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B35" s="22" t="s">
+    <row r="35" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B35" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="C35" s="23">
-        <v>1</v>
-      </c>
-      <c r="D35" s="24" t="s">
+      <c r="C35" s="20">
+        <v>1</v>
+      </c>
+      <c r="D35" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="E35" s="24" t="s">
+      <c r="E35" s="21" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B36" s="22" t="s">
+    <row r="36" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B36" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="C36" s="23">
-        <v>2</v>
-      </c>
-      <c r="D36" s="24" t="s">
+      <c r="C36" s="20">
+        <v>2</v>
+      </c>
+      <c r="D36" s="21" t="s">
         <v>172</v>
       </c>
-      <c r="E36" s="24" t="s">
+      <c r="E36" s="21" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B37" s="22" t="s">
+    <row r="37" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B37" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="C37" s="23">
-        <v>2</v>
-      </c>
-      <c r="D37" s="24" t="s">
+      <c r="C37" s="20">
+        <v>2</v>
+      </c>
+      <c r="D37" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="E37" s="24" t="s">
+      <c r="E37" s="21" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B38" s="22" t="s">
+    <row r="38" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B38" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="C38" s="23">
-        <v>1</v>
-      </c>
-      <c r="D38" s="24" t="s">
+      <c r="C38" s="20">
+        <v>1</v>
+      </c>
+      <c r="D38" s="21" t="s">
         <v>174</v>
       </c>
-      <c r="E38" s="24" t="s">
+      <c r="E38" s="21" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B39" s="22" t="s">
+    <row r="39" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B39" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="C39" s="23">
-        <v>1</v>
-      </c>
-      <c r="D39" s="24" t="s">
+      <c r="C39" s="20">
+        <v>1</v>
+      </c>
+      <c r="D39" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="E39" s="24" t="s">
+      <c r="E39" s="21" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B40" s="22" t="s">
+    <row r="40" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B40" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="C40" s="23">
-        <v>1</v>
-      </c>
-      <c r="D40" s="24" t="s">
+      <c r="C40" s="20">
+        <v>1</v>
+      </c>
+      <c r="D40" s="21" t="s">
         <v>175</v>
       </c>
-      <c r="E40" s="24" t="s">
+      <c r="E40" s="21" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B41" s="22" t="s">
+    <row r="41" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B41" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="C41" s="23">
+      <c r="C41" s="20">
         <v>3</v>
       </c>
-      <c r="D41" s="24" t="s">
+      <c r="D41" s="21" t="s">
         <v>176</v>
       </c>
-      <c r="E41" s="24" t="s">
+      <c r="E41" s="21" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B42" s="22" t="s">
+    <row r="42" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B42" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="C42" s="23">
-        <v>1</v>
-      </c>
-      <c r="D42" s="24" t="s">
+      <c r="C42" s="20">
+        <v>1</v>
+      </c>
+      <c r="D42" s="21" t="s">
         <v>177</v>
       </c>
-      <c r="E42" s="24" t="s">
+      <c r="E42" s="21" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B43" s="22" t="s">
+    <row r="43" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B43" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="C43" s="23">
-        <v>1</v>
-      </c>
-      <c r="D43" s="24" t="s">
+      <c r="C43" s="20">
+        <v>1</v>
+      </c>
+      <c r="D43" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="E43" s="24" t="s">
+      <c r="E43" s="21" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B44" s="22" t="s">
+    <row r="44" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B44" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="C44" s="23">
-        <v>2</v>
-      </c>
-      <c r="D44" s="24" t="s">
+      <c r="C44" s="20">
+        <v>2</v>
+      </c>
+      <c r="D44" s="21" t="s">
         <v>179</v>
       </c>
-      <c r="E44" s="24" t="s">
+      <c r="E44" s="21" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B45" s="22" t="s">
+    <row r="45" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B45" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="C45" s="23">
-        <v>1</v>
-      </c>
-      <c r="D45" s="24" t="s">
+      <c r="C45" s="20">
+        <v>1</v>
+      </c>
+      <c r="D45" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="E45" s="24" t="s">
+      <c r="E45" s="21" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B46" s="22" t="s">
+    <row r="46" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B46" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="C46" s="23">
-        <v>2</v>
-      </c>
-      <c r="D46" s="24" t="s">
+      <c r="C46" s="20">
+        <v>2</v>
+      </c>
+      <c r="D46" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="E46" s="24" t="s">
+      <c r="E46" s="21" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B47" s="22" t="s">
+    <row r="47" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B47" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="C47" s="23">
-        <v>2</v>
-      </c>
-      <c r="D47" s="24" t="s">
+      <c r="C47" s="20">
+        <v>2</v>
+      </c>
+      <c r="D47" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="E47" s="24" t="s">
+      <c r="E47" s="21" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B48" s="22" t="s">
+    <row r="48" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B48" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="C48" s="23">
-        <v>2</v>
-      </c>
-      <c r="D48" s="24" t="s">
+      <c r="C48" s="20">
+        <v>2</v>
+      </c>
+      <c r="D48" s="21" t="s">
         <v>183</v>
       </c>
-      <c r="E48" s="24" t="s">
+      <c r="E48" s="21" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B49" s="22" t="s">
+    <row r="49" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B49" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="C49" s="23">
-        <v>1</v>
-      </c>
-      <c r="D49" s="24" t="s">
+      <c r="C49" s="20">
+        <v>1</v>
+      </c>
+      <c r="D49" s="21" t="s">
         <v>184</v>
       </c>
-      <c r="E49" s="24" t="s">
+      <c r="E49" s="21" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>120</v>
       </c>
@@ -4204,19 +4222,19 @@
         <v>186</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F51" t="s">
         <v>187</v>
       </c>
       <c r="G51" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="H51" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>4</v>
       </c>
@@ -4235,11 +4253,11 @@
       <c r="G52" t="s">
         <v>5</v>
       </c>
-      <c r="H52" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H52" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>8</v>
       </c>
@@ -4258,11 +4276,11 @@
       <c r="G53" t="s">
         <v>7</v>
       </c>
-      <c r="H53" s="25">
+      <c r="H53" s="22">
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>11</v>
       </c>
@@ -4281,11 +4299,11 @@
       <c r="G54" t="s">
         <v>12</v>
       </c>
-      <c r="H54" s="25">
+      <c r="H54" s="22">
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>17</v>
       </c>
@@ -4304,22 +4322,22 @@
       <c r="G55" t="s">
         <v>18</v>
       </c>
-      <c r="H55" s="25">
+      <c r="H55" s="22">
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>19</v>
       </c>
       <c r="C56" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D56" s="10" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E56" s="10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F56" t="s">
         <v>128</v>
@@ -4327,11 +4345,11 @@
       <c r="G56" t="s">
         <v>20</v>
       </c>
-      <c r="H56" s="25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H56" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>21</v>
       </c>
@@ -4350,11 +4368,11 @@
       <c r="G57" t="s">
         <v>22</v>
       </c>
-      <c r="H57" s="25">
+      <c r="H57" s="22">
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>23</v>
       </c>
@@ -4373,11 +4391,11 @@
       <c r="G58" t="s">
         <v>24</v>
       </c>
-      <c r="H58" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H58" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>25</v>
       </c>
@@ -4396,11 +4414,11 @@
       <c r="G59" t="s">
         <v>18</v>
       </c>
-      <c r="H59" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H59" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>26</v>
       </c>
@@ -4419,11 +4437,11 @@
       <c r="G60" t="s">
         <v>16</v>
       </c>
-      <c r="H60" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H60" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>29</v>
       </c>
@@ -4442,19 +4460,19 @@
       <c r="G61" t="s">
         <v>7</v>
       </c>
-      <c r="H61" s="25">
+      <c r="H61" s="22">
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>30</v>
       </c>
       <c r="C62" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D62" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>120</v>
@@ -4465,11 +4483,11 @@
       <c r="G62" t="s">
         <v>20</v>
       </c>
-      <c r="H62" s="25">
+      <c r="H62" s="22">
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>34</v>
       </c>
@@ -4477,10 +4495,10 @@
         <v>136</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E63" s="10" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="F63" t="s">
         <v>128</v>
@@ -4488,11 +4506,11 @@
       <c r="G63" t="s">
         <v>20</v>
       </c>
-      <c r="H63" s="25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H63" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>35</v>
       </c>
@@ -4511,11 +4529,11 @@
       <c r="G64" t="s">
         <v>18</v>
       </c>
-      <c r="H64" s="25">
+      <c r="H64" s="22">
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>40</v>
       </c>
@@ -4534,11 +4552,11 @@
       <c r="G65" t="s">
         <v>16</v>
       </c>
-      <c r="H65" s="25">
+      <c r="H65" s="22">
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>41</v>
       </c>
@@ -4557,22 +4575,22 @@
       <c r="G66" t="s">
         <v>22</v>
       </c>
-      <c r="H66" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H66" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>42</v>
       </c>
       <c r="C67" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D67" s="10" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E67" s="10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F67" t="s">
         <v>129</v>
@@ -4580,16 +4598,16 @@
       <c r="G67" t="s">
         <v>12</v>
       </c>
-      <c r="H67" s="25">
+      <c r="H67" s="22">
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>45</v>
       </c>
       <c r="C68" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D68" s="10" t="s">
         <v>133</v>
@@ -4603,11 +4621,11 @@
       <c r="G68" t="s">
         <v>7</v>
       </c>
-      <c r="H68" s="25">
+      <c r="H68" s="22">
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>47</v>
       </c>
@@ -4626,11 +4644,11 @@
       <c r="G69" t="s">
         <v>20</v>
       </c>
-      <c r="H69" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H69" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>49</v>
       </c>
@@ -4638,7 +4656,7 @@
         <v>139</v>
       </c>
       <c r="D70" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E70" s="10" t="s">
         <v>124</v>
@@ -4649,22 +4667,22 @@
       <c r="G70" t="s">
         <v>16</v>
       </c>
-      <c r="H70" s="25">
+      <c r="H70" s="22">
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>50</v>
       </c>
       <c r="C71" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D71" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E71" s="10" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F71" t="s">
         <v>129</v>
@@ -4672,11 +4690,11 @@
       <c r="G71" t="s">
         <v>12</v>
       </c>
-      <c r="H71" s="25">
+      <c r="H71" s="22">
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>51</v>
       </c>
@@ -4687,7 +4705,7 @@
         <v>132</v>
       </c>
       <c r="E72" s="10" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F72" t="s">
         <v>129</v>
@@ -4695,22 +4713,22 @@
       <c r="G72" t="s">
         <v>28</v>
       </c>
-      <c r="H72" s="25">
+      <c r="H72" s="22">
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>52</v>
       </c>
       <c r="C73" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D73" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E73" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F73" t="s">
         <v>128</v>
@@ -4718,19 +4736,19 @@
       <c r="G73" t="s">
         <v>20</v>
       </c>
-      <c r="H73" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H73" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>53</v>
       </c>
       <c r="C74" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D74" s="10" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E74" s="10" t="s">
         <v>120</v>
@@ -4741,16 +4759,16 @@
       <c r="G74" t="s">
         <v>5</v>
       </c>
-      <c r="H74" s="25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H74" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>54</v>
       </c>
       <c r="C75" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D75" s="10" t="s">
         <v>132</v>
@@ -4764,11 +4782,11 @@
       <c r="G75" t="s">
         <v>12</v>
       </c>
-      <c r="H75" s="25">
+      <c r="H75" s="22">
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>55</v>
       </c>
@@ -4787,11 +4805,11 @@
       <c r="G76" t="s">
         <v>14</v>
       </c>
-      <c r="H76" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H76" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>57</v>
       </c>
@@ -4810,11 +4828,11 @@
       <c r="G77" t="s">
         <v>22</v>
       </c>
-      <c r="H77" s="25">
+      <c r="H77" s="22">
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>58</v>
       </c>
@@ -4833,22 +4851,22 @@
       <c r="G78" t="s">
         <v>24</v>
       </c>
-      <c r="H78" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H78" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>60</v>
       </c>
       <c r="C79" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="D79" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E79" s="10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F79" t="s">
         <v>129</v>
@@ -4856,11 +4874,11 @@
       <c r="G79" t="s">
         <v>10</v>
       </c>
-      <c r="H79" s="25">
+      <c r="H79" s="22">
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>61</v>
       </c>
@@ -4879,11 +4897,11 @@
       <c r="G80" t="s">
         <v>62</v>
       </c>
-      <c r="H80" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H80" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>63</v>
       </c>
@@ -4902,11 +4920,11 @@
       <c r="G81" t="s">
         <v>20</v>
       </c>
-      <c r="H81" s="25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H81" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>70</v>
       </c>
@@ -4925,16 +4943,16 @@
       <c r="G82" t="s">
         <v>20</v>
       </c>
-      <c r="H82" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H82" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>71</v>
       </c>
       <c r="C83" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D83" s="10" t="s">
         <v>131</v>
@@ -4948,11 +4966,11 @@
       <c r="G83" t="s">
         <v>28</v>
       </c>
-      <c r="H83" s="25">
+      <c r="H83" s="22">
         <v>4</v>
       </c>
     </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>73</v>
       </c>
@@ -4971,11 +4989,11 @@
       <c r="G84" t="s">
         <v>24</v>
       </c>
-      <c r="H84" s="25">
+      <c r="H84" s="22">
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>75</v>
       </c>
@@ -4994,11 +5012,11 @@
       <c r="G85" t="s">
         <v>18</v>
       </c>
-      <c r="H85" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H85" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>76</v>
       </c>
@@ -5017,22 +5035,22 @@
       <c r="G86" t="s">
         <v>22</v>
       </c>
-      <c r="H86" s="25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H86" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>78</v>
       </c>
       <c r="C87" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D87" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E87" s="10" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F87" t="s">
         <v>127</v>
@@ -5040,22 +5058,22 @@
       <c r="G87" t="s">
         <v>62</v>
       </c>
-      <c r="H87" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="88" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H87" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>84</v>
       </c>
       <c r="C88" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D88" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E88" s="10" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F88" t="s">
         <v>127</v>
@@ -5063,16 +5081,16 @@
       <c r="G88" t="s">
         <v>7</v>
       </c>
-      <c r="H88" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="89" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H88" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>85</v>
       </c>
       <c r="C89" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D89" s="10" t="s">
         <v>132</v>
@@ -5086,11 +5104,11 @@
       <c r="G89" t="s">
         <v>62</v>
       </c>
-      <c r="H89" s="25">
+      <c r="H89" s="22">
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
         <v>86</v>
       </c>
@@ -5109,16 +5127,16 @@
       <c r="G90" t="s">
         <v>24</v>
       </c>
-      <c r="H90" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="91" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H90" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
         <v>87</v>
       </c>
       <c r="C91" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D91" s="10" t="s">
         <v>132</v>
@@ -5132,11 +5150,11 @@
       <c r="G91" t="s">
         <v>62</v>
       </c>
-      <c r="H91" s="25">
+      <c r="H91" s="22">
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
         <v>89</v>
       </c>
@@ -5155,11 +5173,11 @@
       <c r="G92" t="s">
         <v>5</v>
       </c>
-      <c r="H92" s="25">
+      <c r="H92" s="22">
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
         <v>90</v>
       </c>
@@ -5170,7 +5188,7 @@
         <v>131</v>
       </c>
       <c r="E93" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F93" t="s">
         <v>127</v>
@@ -5178,11 +5196,11 @@
       <c r="G93" t="s">
         <v>62</v>
       </c>
-      <c r="H93" s="25">
+      <c r="H93" s="22">
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
         <v>95</v>
       </c>
@@ -5201,11 +5219,11 @@
       <c r="G94" t="s">
         <v>20</v>
       </c>
-      <c r="H94" s="25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H94" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
         <v>97</v>
       </c>
@@ -5224,19 +5242,19 @@
       <c r="G95" t="s">
         <v>24</v>
       </c>
-      <c r="H95" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="96" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H95" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
         <v>100</v>
       </c>
       <c r="C96" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D96" s="10" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E96" s="10" t="s">
         <v>121</v>
@@ -5247,11 +5265,11 @@
       <c r="G96" t="s">
         <v>14</v>
       </c>
-      <c r="H96" s="25">
+      <c r="H96" s="22">
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
         <v>101</v>
       </c>
@@ -5270,11 +5288,11 @@
       <c r="G97" t="s">
         <v>24</v>
       </c>
-      <c r="H97" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="98" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H97" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
         <v>102</v>
       </c>
@@ -5293,11 +5311,11 @@
       <c r="G98" t="s">
         <v>14</v>
       </c>
-      <c r="H98" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="99" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H98" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
         <v>104</v>
       </c>
@@ -5316,22 +5334,22 @@
       <c r="G99" t="s">
         <v>28</v>
       </c>
-      <c r="H99" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="100" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H99" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
         <v>105</v>
       </c>
       <c r="C100" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D100" s="10" t="s">
         <v>132</v>
       </c>
       <c r="E100" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F100" t="s">
         <v>128</v>
@@ -5339,11 +5357,11 @@
       <c r="G100" t="s">
         <v>20</v>
       </c>
-      <c r="H100" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="101" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H100" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
         <v>106</v>
       </c>
@@ -5362,11 +5380,11 @@
       <c r="G101" t="s">
         <v>24</v>
       </c>
-      <c r="H101" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="102" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H101" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
         <v>107</v>
       </c>
@@ -5385,11 +5403,11 @@
       <c r="G102" t="s">
         <v>22</v>
       </c>
-      <c r="H102" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="103" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H102" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
         <v>109</v>
       </c>
@@ -5408,11 +5426,11 @@
       <c r="G103" t="s">
         <v>24</v>
       </c>
-      <c r="H103" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="104" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H103" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
         <v>110</v>
       </c>
@@ -5431,19 +5449,19 @@
       <c r="G104" t="s">
         <v>16</v>
       </c>
-      <c r="H104" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="105" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H104" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
         <v>114</v>
       </c>
       <c r="C105" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D105" s="10" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E105" s="10" t="s">
         <v>124</v>
@@ -5454,7 +5472,7 @@
       <c r="G105" t="s">
         <v>16</v>
       </c>
-      <c r="H105" s="25">
+      <c r="H105" s="22">
         <v>3</v>
       </c>
     </row>
@@ -5468,37 +5486,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A3:M24"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="116" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView zoomScale="116" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="16" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
+    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
         <v>131</v>
       </c>
       <c r="B4" s="10" t="s">
@@ -5517,47 +5535,47 @@
         <v>195</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
+    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
         <v>132</v>
       </c>
       <c r="B5" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="D5" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="E5" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="F5" s="11" t="s">
         <v>204</v>
       </c>
-      <c r="F5" s="11" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="19" t="s">
+    </row>
+    <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
         <v>133</v>
       </c>
       <c r="B6" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="E6" s="12" t="s">
         <v>212</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="F6" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="E6" s="12" t="s">
-        <v>214</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
@@ -5571,232 +5589,232 @@
       <c r="L7" s="10"/>
       <c r="M7" s="10"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>190</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="E9" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="F9" s="21" t="s">
+      <c r="F9" s="16" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="18" t="s">
+    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
         <v>131</v>
       </c>
       <c r="B10" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>302</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="F12" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>199</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>209</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>216</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>217</v>
-      </c>
-      <c r="D12" s="12" t="s">
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
         <v>218</v>
       </c>
-      <c r="E12" s="12" t="s">
-        <v>219</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="15" t="s">
-        <v>221</v>
-      </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E15" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="F15" s="17" t="s">
+      <c r="F15" s="16" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="18" t="s">
+    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
         <v>131</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="10" t="s">
-        <v>223</v>
+        <v>296</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="E16" s="10"/>
-      <c r="F16" s="11" t="s">
+      <c r="F16" s="11"/>
+    </row>
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>297</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>232</v>
-      </c>
       <c r="D17" s="10" t="s">
-        <v>233</v>
+        <v>298</v>
       </c>
       <c r="E17" s="10"/>
-      <c r="F17" s="11"/>
-    </row>
-    <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="19" t="s">
+      <c r="F17" s="11" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
         <v>133</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
-        <v>239</v>
+        <v>299</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="F18" s="13"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="15" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="B22" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="B21" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="E21" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="F21" s="17" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="B22" s="10" t="s">
+      <c r="C22" s="10" t="s">
+        <v>303</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="B23" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C23" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D23" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="E23" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="E22" s="10" t="s">
-        <v>229</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="B23" s="10" t="s">
+      <c r="F23" s="11" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>306</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="E24" s="12" t="s">
         <v>234</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="F24" s="13" t="s">
         <v>235</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>236</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>237</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="B24" s="12" t="s">
-        <v>242</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>243</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>244</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>245</v>
-      </c>
-      <c r="F24" s="13" t="s">
-        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -5809,81 +5827,83 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:O50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="114" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="114" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
-        <v>247</v>
-      </c>
-      <c r="B1" s="16" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="16" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
+    <row r="2" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
         <v>131</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10" t="s">
-        <v>249</v>
+        <v>307</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="F2" s="11"/>
     </row>
-    <row r="3" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
+    <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
         <v>132</v>
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="10" t="s">
-        <v>254</v>
-      </c>
-      <c r="D3" s="10"/>
+        <v>243</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>245</v>
+      </c>
       <c r="E3" s="10"/>
       <c r="F3" s="11" t="s">
-        <v>255</v>
+        <v>308</v>
       </c>
       <c r="I3" s="10"/>
     </row>
-    <row r="4" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="19" t="s">
+    <row r="4" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
         <v>133</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="13"/>
       <c r="I4" s="10"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
@@ -5892,99 +5912,101 @@
       <c r="F5" s="10"/>
       <c r="I5" s="10"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I6" s="10"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="15" t="s">
-        <v>248</v>
-      </c>
-      <c r="B7" s="16" t="s">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="B7" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="16" t="s">
         <v>139</v>
       </c>
       <c r="I7" s="10"/>
     </row>
-    <row r="8" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="18" t="s">
+    <row r="8" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
         <v>131</v>
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
       <c r="D8" s="10" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="E8" s="10"/>
       <c r="F8" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="I8" s="10"/>
+    </row>
+    <row r="9" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>309</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="I9" s="10"/>
+    </row>
+    <row r="10" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12" t="s">
         <v>253</v>
       </c>
-      <c r="I8" s="10"/>
-    </row>
-    <row r="9" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>256</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>258</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="F9" s="11"/>
-      <c r="I9" s="10"/>
-    </row>
-    <row r="10" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12" t="s">
-        <v>263</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>264</v>
-      </c>
-      <c r="E10" s="12"/>
+      <c r="E10" s="12" t="s">
+        <v>242</v>
+      </c>
       <c r="F10" s="13"/>
       <c r="I10" s="10"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I11" s="10"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="15" t="s">
-        <v>265</v>
-      </c>
-      <c r="B12" s="16" t="s">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>254</v>
+      </c>
+      <c r="B12" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="F12" s="16" t="s">
         <v>139</v>
       </c>
       <c r="I12" s="10"/>
@@ -5995,321 +6017,329 @@
       <c r="N12" s="10"/>
       <c r="O12" s="10"/>
     </row>
-    <row r="13" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="18" t="s">
+    <row r="13" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
         <v>131</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>268</v>
+        <v>244</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="F13" s="11"/>
       <c r="I13" s="10"/>
     </row>
-    <row r="14" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="18" t="s">
+    <row r="14" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
         <v>132</v>
       </c>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
+      <c r="D14" s="10" t="s">
+        <v>256</v>
+      </c>
       <c r="E14" s="10"/>
-      <c r="F14" s="11" t="s">
-        <v>274</v>
-      </c>
+      <c r="F14" s="11"/>
       <c r="I14" s="10"/>
     </row>
-    <row r="15" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="19" t="s">
+    <row r="15" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
         <v>133</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>278</v>
-      </c>
-      <c r="D15" s="12"/>
+        <v>267</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>310</v>
+      </c>
       <c r="E15" s="12" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="F15" s="13"/>
       <c r="I15" s="10"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I16" s="10"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A17" s="15" t="s">
-        <v>266</v>
-      </c>
-      <c r="B17" s="16" t="s">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="B17" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D17" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="E17" s="16" t="s">
+      <c r="E17" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="F17" s="17" t="s">
+      <c r="F17" s="16" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="18" t="s">
+    <row r="18" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
         <v>131</v>
       </c>
       <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
+      <c r="C18" s="10" t="s">
+        <v>248</v>
+      </c>
       <c r="D18" s="10" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>272</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="18" t="s">
+        <v>261</v>
+      </c>
+      <c r="F18" s="11"/>
+    </row>
+    <row r="19" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="17" t="s">
         <v>132</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
-      <c r="F19" s="11"/>
-    </row>
-    <row r="20" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="19" t="s">
+      <c r="F19" s="11" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="B20" s="12" t="s">
-        <v>280</v>
-      </c>
-      <c r="C20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12" t="s">
+        <v>238</v>
+      </c>
       <c r="D20" s="12"/>
       <c r="E20" s="12" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A22" s="15" t="s">
-        <v>283</v>
-      </c>
-      <c r="B22" s="16" t="s">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
+        <v>272</v>
+      </c>
+      <c r="B22" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="C22" s="16" t="s">
+      <c r="C22" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="D22" s="16" t="s">
+      <c r="D22" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="E22" s="16" t="s">
+      <c r="E22" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="F22" s="17" t="s">
+      <c r="F22" s="16" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="18" t="s">
+    <row r="23" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="B23" s="10"/>
+      <c r="B23" s="10" t="s">
+        <v>276</v>
+      </c>
       <c r="C23" s="10" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
       <c r="F23" s="11" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="18" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="17" t="s">
         <v>132</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="10" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="F24" s="11"/>
     </row>
-    <row r="25" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="19" t="s">
+    <row r="25" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="18" t="s">
         <v>133</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
       <c r="D25" s="12" t="s">
-        <v>296</v>
+        <v>311</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="F25" s="13" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="N26" s="9"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A27" s="15" t="s">
-        <v>284</v>
-      </c>
-      <c r="B27" s="16" t="s">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="14" t="s">
+        <v>273</v>
+      </c>
+      <c r="B27" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="D27" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="E27" s="16" t="s">
+      <c r="E27" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="F27" s="17" t="s">
+      <c r="F27" s="16" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="18" t="s">
+    <row r="28" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="17" t="s">
         <v>131</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>287</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>288</v>
-      </c>
+        <v>312</v>
+      </c>
+      <c r="C28" s="10"/>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
-      <c r="F28" s="11"/>
+      <c r="F28" s="11" t="s">
+        <v>289</v>
+      </c>
       <c r="G28" s="10"/>
     </row>
-    <row r="29" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="18" t="s">
+    <row r="29" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="17" t="s">
         <v>132</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>295</v>
-      </c>
-      <c r="F29" s="11"/>
-    </row>
-    <row r="30" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A30" s="19" t="s">
+        <v>281</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="18" t="s">
         <v>133</v>
       </c>
       <c r="B30" s="12"/>
       <c r="C30" s="12" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="D30" s="12"/>
       <c r="E30" s="12"/>
       <c r="F30" s="13" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="I31" s="27" t="s">
-        <v>302</v>
-      </c>
-      <c r="J31" s="26" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="I32" s="29" t="s">
-        <v>247</v>
-      </c>
-      <c r="J32" s="30" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="33" spans="9:10" x14ac:dyDescent="0.3">
-      <c r="I33" s="29" t="s">
-        <v>248</v>
-      </c>
-      <c r="J33" s="30" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="34" spans="9:10" x14ac:dyDescent="0.3">
-      <c r="I34" s="29" t="s">
-        <v>265</v>
-      </c>
-      <c r="J34" s="30" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="35" spans="9:10" x14ac:dyDescent="0.3">
-      <c r="I35" s="29" t="s">
-        <v>266</v>
-      </c>
-      <c r="J35" s="30" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="36" spans="9:10" x14ac:dyDescent="0.3">
-      <c r="I36" s="29" t="s">
-        <v>283</v>
-      </c>
-      <c r="J36" s="30" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="37" spans="9:10" x14ac:dyDescent="0.3">
-      <c r="I37" s="28" t="s">
-        <v>284</v>
-      </c>
-      <c r="J37" s="30" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="50" spans="11:11" x14ac:dyDescent="0.3">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="I31" s="24" t="s">
+        <v>291</v>
+      </c>
+      <c r="J31" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I32" s="26" t="s">
+        <v>236</v>
+      </c>
+      <c r="J32" s="27" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="33" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I33" s="26" t="s">
+        <v>237</v>
+      </c>
+      <c r="J33" s="27" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="34" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I34" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="J34" s="27" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="35" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I35" s="26" t="s">
+        <v>255</v>
+      </c>
+      <c r="J35" s="27" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="36" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I36" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="J36" s="27" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="37" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I37" s="25" t="s">
+        <v>273</v>
+      </c>
+      <c r="J37" s="27" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="50" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K50" s="9"/>
     </row>
   </sheetData>

</xml_diff>